<commit_message>
added strategy for attacks
</commit_message>
<xml_diff>
--- a/docs/dice_roll_odds.xlsx
+++ b/docs/dice_roll_odds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo Carvalho\Documents\GitHub\AIAD1819\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C12AC5D-2BB6-4067-835F-761FF2807C3C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C16F3C-2D65-41C8-B8BC-B66C293F15C1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" xr2:uid="{E372DD10-806D-4464-8FF0-76EF9731FE20}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>Attacker</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>Nunca compensa</t>
+  </si>
+  <si>
+    <t>Só 'compensa' se apenas tiver 2 unidades na origem</t>
+  </si>
+  <si>
+    <t>Compensa se o defensor tiver apenas 2 unidades (assumir que não lança dois dados)</t>
+  </si>
+  <si>
+    <t>Compensa sempre que possivel</t>
   </si>
 </sst>
 </file>
@@ -124,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -143,9 +152,91 @@
     </border>
     <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -155,10 +246,67 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -166,9 +314,11 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -177,59 +327,11 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -238,42 +340,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -591,320 +735,323 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1AC4BE6-6F98-47A9-AD22-5B81133252AF}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="76.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="4" max="5" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="72.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="72.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="7" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18" t="s">
+      <c r="F3" s="13"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11">
+      <c r="G4" s="2"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="17">
         <v>0.40400000000000003</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="18">
         <v>1</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="19">
         <v>1</v>
       </c>
-      <c r="F5" s="13">
-        <f>1-C5</f>
+      <c r="F5" s="20">
+        <f t="shared" ref="F5:F10" si="0">1-C5</f>
         <v>0.59599999999999997</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="20" t="s">
+      <c r="G5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="21">
         <v>0.26700000000000002</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="22">
         <v>1</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="23">
         <v>2</v>
       </c>
-      <c r="F6" s="17">
-        <f>1-C6</f>
+      <c r="F6" s="24">
+        <f t="shared" si="0"/>
         <v>0.73299999999999998</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="5" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="25">
         <v>0.6</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="26">
         <v>2</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="27">
         <v>1</v>
       </c>
-      <c r="F7" s="4">
-        <f>1-C7</f>
+      <c r="F7" s="28">
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="22" t="s">
+      <c r="G7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="H7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="25">
         <v>0.38400000000000001</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="26">
         <v>2</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="27">
         <v>2</v>
       </c>
-      <c r="F8" s="4">
-        <f>1-C8</f>
+      <c r="F8" s="28">
+        <f t="shared" si="0"/>
         <v>0.61599999999999999</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="22" t="s">
+      <c r="G8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="H8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="25">
         <v>0.65</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="26">
         <v>3</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="27">
         <v>1</v>
       </c>
-      <c r="F9" s="4">
-        <f>1-C9</f>
+      <c r="F9" s="28">
+        <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="22" t="s">
+      <c r="G9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="H9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3">
+      <c r="B10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="25">
         <v>0.53600000000000003</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="26">
         <v>3</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="27">
         <v>2</v>
       </c>
-      <c r="F10" s="4">
-        <f>1-C10</f>
+      <c r="F10" s="28">
+        <f t="shared" si="0"/>
         <v>0.46399999999999997</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="19" t="s">
+      <c r="G10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="H10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H5:H6"/>
+  <mergeCells count="7">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>